<commit_message>
TC  2 3 4 5 6 7 8 9 Updated
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurud\OneDrive\Documents\UiPath\M3TECH_POC\Testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurud\OneDrive\Documents\UiPath\M3TECH_POC\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D7EA3F-111B-493E-8810-60A156D90A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD922A1-CB49-4FCA-B8AB-C687F01F34B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
   <si>
     <t>TestCase</t>
   </si>
@@ -97,6 +97,9 @@
     <t>Co_App_Downpay</t>
   </si>
   <si>
+    <t>Co_App_Gift_Description</t>
+  </si>
+  <si>
     <t>Co_App_Gift_assetvalue</t>
   </si>
   <si>
@@ -142,9 +145,6 @@
     <t>Co_App_Payment</t>
   </si>
   <si>
-    <t>Co_App_MaturityDate</t>
-  </si>
-  <si>
     <t>Co_App_Lia_Description</t>
   </si>
   <si>
@@ -193,6 +193,9 @@
     <t>RRSP</t>
   </si>
   <si>
+    <t>Gift</t>
+  </si>
+  <si>
     <t>C128</t>
   </si>
   <si>
@@ -298,6 +301,9 @@
     <t>C73</t>
   </si>
   <si>
+    <t>C144</t>
+  </si>
+  <si>
     <t>TestCases</t>
   </si>
   <si>
@@ -371,18 +377,14 @@
   </si>
   <si>
     <t>autoboss</t>
-  </si>
-  <si>
-    <t>C144</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -439,7 +441,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -449,10 +450,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -675,34 +679,33 @@
   </sheetPr>
   <dimension ref="A1:AQ15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="10" width="25.77734375" customWidth="1"/>
-    <col min="11" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" customWidth="1"/>
-    <col min="16" max="17" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="7" width="25.77734375" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" customWidth="1"/>
+    <col min="9" max="10" width="25.77734375" customWidth="1"/>
+    <col min="11" max="14" width="15.6640625" customWidth="1"/>
+    <col min="15" max="17" width="15.44140625" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
     <col min="19" max="19" width="19.6640625" customWidth="1"/>
     <col min="20" max="20" width="18.88671875" customWidth="1"/>
     <col min="21" max="21" width="21.44140625" customWidth="1"/>
     <col min="22" max="22" width="16.109375" customWidth="1"/>
-    <col min="23" max="24" width="19.33203125" customWidth="1"/>
-    <col min="25" max="25" width="21.21875" customWidth="1"/>
-    <col min="26" max="26" width="19.33203125" customWidth="1"/>
-    <col min="27" max="27" width="23.6640625" customWidth="1"/>
-    <col min="28" max="28" width="23.21875" customWidth="1"/>
-    <col min="29" max="29" width="22.6640625" customWidth="1"/>
-    <col min="30" max="31" width="24.77734375" customWidth="1"/>
-    <col min="35" max="35" width="14.33203125" customWidth="1"/>
+    <col min="23" max="25" width="19.33203125" customWidth="1"/>
+    <col min="26" max="26" width="21.21875" customWidth="1"/>
+    <col min="27" max="27" width="19.33203125" customWidth="1"/>
+    <col min="28" max="28" width="23.6640625" customWidth="1"/>
+    <col min="29" max="29" width="23.21875" customWidth="1"/>
+    <col min="30" max="30" width="22.6640625" customWidth="1"/>
+    <col min="31" max="32" width="24.77734375" customWidth="1"/>
+    <col min="36" max="36" width="14.33203125" customWidth="1"/>
+    <col min="41" max="41" width="17.109375" customWidth="1"/>
     <col min="42" max="42" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -800,7 +803,7 @@
       <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
@@ -809,22 +812,22 @@
       <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AO1" s="2" t="s">
@@ -850,7 +853,6 @@
       <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AN2" s="5"/>
     </row>
     <row r="3" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -871,10 +873,10 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -910,11 +912,11 @@
       <c r="N4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>20000</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
       <c r="R4" s="1">
         <v>30000</v>
       </c>
@@ -924,27 +926,30 @@
       <c r="V4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="5">
         <v>20000</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="5">
         <v>30000</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="5">
         <v>10000</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="AA4" s="5">
         <v>20000</v>
       </c>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
     </row>
     <row r="5" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -968,14 +973,20 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="6">
+      <c r="L5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="3">
+        <v>30000</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="5">
         <v>20000</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="1">
         <v>30000</v>
       </c>
@@ -985,24 +996,27 @@
       <c r="V5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="5">
         <v>20000</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="5">
         <v>30000</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z5" s="5">
         <v>10000</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AA5" s="1">
         <v>20000</v>
       </c>
-      <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
     </row>
     <row r="6" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>44</v>
@@ -1023,15 +1037,15 @@
         <v>52</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="K6" s="5"/>
       <c r="L6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1039,13 +1053,13 @@
         <v>30000</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O6" s="1">
         <v>100000</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q6" s="1">
         <v>40000</v>
@@ -1054,27 +1068,30 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="AA6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1" t="s">
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AB6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AD6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE6" s="1">
+      <c r="AF6" s="1">
         <v>50000</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>44</v>
@@ -1104,13 +1121,13 @@
         <v>30000</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O7" s="1">
         <v>100000</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q7" s="1">
         <v>40000</v>
@@ -1118,16 +1135,16 @@
       <c r="S7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="5">
         <v>20000</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="5">
         <v>30000</v>
       </c>
     </row>
     <row r="8" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>44</v>
@@ -1150,41 +1167,38 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="AF8" s="1">
+      <c r="AG8" s="1">
         <v>5000</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AH8" s="1">
         <v>500</v>
       </c>
-      <c r="AH8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AI8" s="1" t="s">
-        <v>66</v>
+      <c r="AI8" s="1">
+        <v>100</v>
       </c>
       <c r="AJ8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AK8" s="1">
+      <c r="AK8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL8" s="1">
         <v>7000</v>
       </c>
-      <c r="AL8" s="1">
+      <c r="AM8" s="1">
         <v>700</v>
       </c>
-      <c r="AM8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AN8" s="5">
-        <v>44663</v>
+      <c r="AN8" s="1">
+        <v>100</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AQ8" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
@@ -1197,6 +1211,7 @@
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="K14" s="3"/>
@@ -1214,17 +1229,17 @@
     </row>
     <row r="15" spans="1:43" ht="13.2" x14ac:dyDescent="0.25">
       <c r="K15" s="3"/>
-      <c r="L15" s="6"/>
+      <c r="L15" s="5"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="6"/>
+      <c r="N15" s="5"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="6"/>
+      <c r="P15" s="5"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1238,198 +1253,209 @@
   </sheetPr>
   <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
     <col min="13" max="13" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
+      <c r="M1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="9">
+      <c r="D2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="8">
         <v>16502</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="7">
+      <c r="G2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="6">
         <v>110</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="L2" s="9">
+      <c r="K2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="8">
         <v>16502</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
+      <c r="M2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-    </row>
-    <row r="4" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>116</v>
+        <v>92</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1444,48 +1470,46 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>101</v>
       </c>
@@ -1493,7 +1517,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>103</v>
       </c>
@@ -1501,7 +1525,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>105</v>
       </c>
@@ -1509,7 +1533,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
@@ -1517,7 +1541,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>109</v>
       </c>
@@ -1525,7 +1549,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>111</v>
       </c>
@@ -1533,12 +1557,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1559,18 +1583,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comment to test case 10
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -220,7 +220,7 @@
     <t>C1102</t>
   </si>
   <si>
-    <t>100.00</t>
+    <t>100.0</t>
   </si>
   <si>
     <t>Credit Card</t>
@@ -247,9 +247,6 @@
     <t>CoApplicantLastname</t>
   </si>
   <si>
-    <t>DOB</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -262,10 +259,10 @@
     <t>city</t>
   </si>
   <si>
-    <t>postalcode</t>
+    <t>Province</t>
   </si>
   <si>
-    <t>AuthorizatioDate</t>
+    <t>postalcode</t>
   </si>
   <si>
     <t>AuthorizationMethod</t>
@@ -331,7 +328,10 @@
     <t>Toronto</t>
   </si>
   <si>
-    <t>M2N6S6</t>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>M2N6S1</t>
   </si>
   <si>
     <t>Credit Bureau</t>
@@ -422,9 +422,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
-  </numFmts>
   <fonts count="10">
     <font>
       <sz val="10.0"/>
@@ -502,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -547,9 +544,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -50026,20 +50020,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="6" width="22.75"/>
-    <col customWidth="1" min="14" max="14" width="17.38"/>
-    <col customWidth="1" min="15" max="15" width="17.63"/>
-    <col customWidth="1" min="16" max="16" width="22.0"/>
-    <col customWidth="1" min="17" max="17" width="17.88"/>
-    <col customWidth="1" min="18" max="18" width="17.38"/>
-    <col customWidth="1" min="19" max="19" width="18.25"/>
-    <col customWidth="1" min="20" max="20" width="23.25"/>
-    <col customWidth="1" min="21" max="21" width="24.75"/>
-    <col customWidth="1" min="22" max="22" width="25.88"/>
-    <col customWidth="1" min="23" max="23" width="27.63"/>
-    <col customWidth="1" min="24" max="24" width="22.5"/>
-    <col customWidth="1" min="25" max="25" width="23.63"/>
-    <col customWidth="1" min="26" max="26" width="22.13"/>
-    <col customWidth="1" min="27" max="27" width="24.0"/>
+    <col customWidth="1" min="14" max="14" width="17.63"/>
+    <col customWidth="1" min="15" max="15" width="22.0"/>
+    <col customWidth="1" min="16" max="16" width="17.88"/>
+    <col customWidth="1" min="17" max="17" width="17.38"/>
+    <col customWidth="1" min="18" max="18" width="18.25"/>
+    <col customWidth="1" min="19" max="19" width="23.25"/>
+    <col customWidth="1" min="20" max="20" width="24.75"/>
+    <col customWidth="1" min="21" max="21" width="25.88"/>
+    <col customWidth="1" min="22" max="22" width="27.63"/>
+    <col customWidth="1" min="23" max="23" width="22.5"/>
+    <col customWidth="1" min="24" max="24" width="23.63"/>
+    <col customWidth="1" min="25" max="25" width="22.13"/>
+    <col customWidth="1" min="26" max="26" width="24.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -50062,10 +50055,10 @@
         <v>76</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>78</v>
@@ -50121,9 +50114,7 @@
       <c r="Z1" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
@@ -50137,34 +50128,33 @@
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
       <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>100</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="15">
-        <v>16502.0</v>
+      <c r="G2" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="13">
+        <v>110.0</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="J2" s="13">
-        <v>110.0</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>103</v>
@@ -50175,24 +50165,22 @@
       <c r="M2" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="15">
-        <v>16502.0</v>
-      </c>
-      <c r="O2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
@@ -50206,7 +50194,6 @@
       <c r="AL2" s="8"/>
       <c r="AM2" s="8"/>
       <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
@@ -50227,44 +50214,43 @@
       <c r="F3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
       <c r="AA3" s="16"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17"/>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="17"/>
-      <c r="AM3" s="17"/>
-      <c r="AN3" s="17"/>
-      <c r="AO3" s="17"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
     </row>
     <row r="4">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>108</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -50276,67 +50262,66 @@
       <c r="D4" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="20">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19">
         <v>5000.0</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="P4" s="19">
         <v>500.0</v>
       </c>
-      <c r="R4" s="20">
+      <c r="Q4" s="19">
         <v>100.0</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="R4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="T4" s="20">
+      <c r="S4" s="19">
         <v>10000.0</v>
       </c>
-      <c r="U4" s="20">
+      <c r="T4" s="19">
         <v>1000.0</v>
       </c>
-      <c r="V4" s="20">
+      <c r="U4" s="19">
         <v>100.0</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="V4" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="X4" s="20">
+      <c r="W4" s="19">
         <v>8000.0</v>
       </c>
-      <c r="Y4" s="20">
+      <c r="X4" s="19">
         <v>800.0</v>
       </c>
-      <c r="Z4" s="20">
+      <c r="Y4" s="19">
         <v>100.0</v>
       </c>
-      <c r="AA4" s="21" t="s">
+      <c r="Z4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="19"/>
-      <c r="AI4" s="19"/>
-      <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-      <c r="AL4" s="19"/>
-      <c r="AM4" s="19"/>
-      <c r="AN4" s="19"/>
-      <c r="AO4" s="19"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -50357,367 +50342,367 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
     </row>
     <row r="2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
     </row>
     <row r="3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
     </row>
     <row r="4">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
     </row>
     <row r="5">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
     </row>
     <row r="6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
     </row>
     <row r="7">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-      <c r="AA7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
     </row>
     <row r="8">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
     </row>
     <row r="9">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="25"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
     </row>
     <row r="10">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
     </row>
     <row r="11">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -50767,36 +50752,36 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Project published to version 10 and test sheet updated
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -433,16 +433,16 @@
     <t>Testcases\TC-8</t>
   </si>
   <si>
+    <t>TC-9</t>
+  </si>
+  <si>
+    <t>Testcases\TC-9</t>
+  </si>
+  <si>
     <t>TC-10</t>
   </si>
   <si>
     <t>Testcases\TC-10</t>
-  </si>
-  <si>
-    <t>TC-9</t>
-  </si>
-  <si>
-    <t>Testcases\TC-9</t>
   </si>
   <si>
     <t>username</t>

</xml_diff>

<commit_message>
try-catch changes in all test cases
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="148">
   <si>
     <t>TestCase</t>
   </si>
@@ -265,6 +265,9 @@
     <t>city</t>
   </si>
   <si>
+    <t>Province</t>
+  </si>
+  <si>
     <t>postalcode</t>
   </si>
   <si>
@@ -365,6 +368,9 @@
   </si>
   <si>
     <t>Toronto</t>
+  </si>
+  <si>
+    <t>Ontario</t>
   </si>
   <si>
     <t>M2N6S6</t>
@@ -50065,28 +50071,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="6" width="22.75"/>
-    <col customWidth="1" min="14" max="14" width="17.63"/>
-    <col customWidth="1" min="15" max="15" width="22.0"/>
-    <col customWidth="1" min="16" max="16" width="17.88"/>
-    <col customWidth="1" min="17" max="17" width="17.38"/>
-    <col customWidth="1" min="18" max="18" width="18.25"/>
-    <col customWidth="1" min="19" max="19" width="23.25"/>
-    <col customWidth="1" min="20" max="20" width="24.75"/>
-    <col customWidth="1" min="21" max="21" width="25.88"/>
-    <col customWidth="1" min="22" max="22" width="27.63"/>
-    <col customWidth="1" min="23" max="23" width="22.5"/>
-    <col customWidth="1" min="24" max="24" width="23.63"/>
-    <col customWidth="1" min="25" max="25" width="22.13"/>
-    <col customWidth="1" min="26" max="26" width="24.0"/>
-    <col customWidth="1" min="28" max="28" width="22.13"/>
-    <col customWidth="1" min="29" max="29" width="24.25"/>
-    <col customWidth="1" min="30" max="30" width="22.75"/>
-    <col customWidth="1" min="34" max="34" width="21.38"/>
-    <col customWidth="1" min="35" max="35" width="22.38"/>
-    <col customWidth="1" min="36" max="36" width="17.38"/>
-    <col customWidth="1" min="37" max="37" width="19.13"/>
-    <col customWidth="1" min="38" max="38" width="22.63"/>
-    <col customWidth="1" min="39" max="39" width="24.5"/>
+    <col customWidth="1" min="15" max="15" width="17.63"/>
+    <col customWidth="1" min="16" max="16" width="22.0"/>
+    <col customWidth="1" min="17" max="17" width="17.88"/>
+    <col customWidth="1" min="18" max="18" width="17.38"/>
+    <col customWidth="1" min="19" max="19" width="18.25"/>
+    <col customWidth="1" min="20" max="20" width="23.25"/>
+    <col customWidth="1" min="21" max="21" width="24.75"/>
+    <col customWidth="1" min="22" max="22" width="25.88"/>
+    <col customWidth="1" min="23" max="23" width="27.63"/>
+    <col customWidth="1" min="24" max="24" width="22.5"/>
+    <col customWidth="1" min="25" max="25" width="23.63"/>
+    <col customWidth="1" min="26" max="26" width="22.13"/>
+    <col customWidth="1" min="27" max="27" width="24.0"/>
+    <col customWidth="1" min="29" max="29" width="22.13"/>
+    <col customWidth="1" min="30" max="30" width="24.25"/>
+    <col customWidth="1" min="31" max="31" width="22.75"/>
+    <col customWidth="1" min="35" max="35" width="21.38"/>
+    <col customWidth="1" min="36" max="36" width="22.38"/>
+    <col customWidth="1" min="37" max="37" width="17.38"/>
+    <col customWidth="1" min="38" max="38" width="19.13"/>
+    <col customWidth="1" min="39" max="39" width="22.63"/>
+    <col customWidth="1" min="40" max="40" width="24.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -50207,20 +50213,23 @@
       <c r="AM1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="AN1" s="5"/>
+      <c r="AN1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -50229,30 +50238,32 @@
         <v>16502.0</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K2" s="13">
         <v>110.0</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="15">
         <v>16502.0</v>
       </c>
-      <c r="P2" s="13" t="s">
-        <v>118</v>
+      <c r="Q2" s="13" t="s">
+        <v>120</v>
       </c>
-      <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
@@ -50275,11 +50286,12 @@
       <c r="AK2" s="16"/>
       <c r="AL2" s="16"/>
       <c r="AM2" s="16"/>
-      <c r="AN2" s="8"/>
+      <c r="AN2" s="16"/>
+      <c r="AO2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>45</v>
@@ -50329,11 +50341,12 @@
       <c r="AK3" s="16"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="16"/>
-      <c r="AN3" s="17"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="17"/>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>45</v>
@@ -50353,78 +50366,79 @@
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="21"/>
-      <c r="Q4" s="22">
+      <c r="Q4" s="21"/>
+      <c r="R4" s="22">
         <v>5000.0</v>
       </c>
-      <c r="R4" s="22">
+      <c r="S4" s="22">
         <v>500.0</v>
       </c>
-      <c r="S4" s="22">
+      <c r="T4" s="22">
         <v>100.0</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="U4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="U4" s="22">
+      <c r="V4" s="22">
         <v>10000.0</v>
       </c>
-      <c r="V4" s="22">
+      <c r="W4" s="22">
         <v>1000.0</v>
       </c>
-      <c r="W4" s="22">
+      <c r="X4" s="22">
         <v>100.0</v>
       </c>
-      <c r="X4" s="19" t="s">
+      <c r="Y4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="Y4" s="22">
+      <c r="Z4" s="22">
         <v>8000.0</v>
       </c>
-      <c r="Z4" s="22">
+      <c r="AA4" s="22">
         <v>800.0</v>
       </c>
-      <c r="AA4" s="22">
+      <c r="AB4" s="22">
         <v>100.0</v>
       </c>
-      <c r="AB4" s="19" t="s">
+      <c r="AC4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="AC4" s="19" t="s">
+      <c r="AD4" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AD4" s="19" t="s">
+      <c r="AE4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="AE4" s="19" t="s">
+      <c r="AF4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AF4" s="22">
+      <c r="AG4" s="22">
         <v>5000.0</v>
       </c>
-      <c r="AG4" s="22">
+      <c r="AH4" s="22">
         <v>500.0</v>
       </c>
-      <c r="AH4" s="22">
+      <c r="AI4" s="22">
         <v>100.0</v>
       </c>
-      <c r="AI4" s="19" t="s">
+      <c r="AJ4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="AJ4" s="22">
+      <c r="AK4" s="22">
         <v>7000.0</v>
       </c>
-      <c r="AK4" s="22">
+      <c r="AL4" s="22">
         <v>700.0</v>
       </c>
-      <c r="AL4" s="22">
+      <c r="AM4" s="22">
         <v>100.0</v>
       </c>
-      <c r="AM4" s="19" t="s">
+      <c r="AN4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="AN4" s="20"/>
+      <c r="AO4" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -50449,10 +50463,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -50482,10 +50496,10 @@
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -50515,10 +50529,10 @@
     </row>
     <row r="3">
       <c r="A3" s="25" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -50548,10 +50562,10 @@
     </row>
     <row r="4">
       <c r="A4" s="25" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
@@ -50581,10 +50595,10 @@
     </row>
     <row r="5">
       <c r="A5" s="25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -50614,10 +50628,10 @@
     </row>
     <row r="6">
       <c r="A6" s="25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -50647,10 +50661,10 @@
     </row>
     <row r="7">
       <c r="A7" s="25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
@@ -50680,10 +50694,10 @@
     </row>
     <row r="8">
       <c r="A8" s="25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -50713,10 +50727,10 @@
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
@@ -50746,10 +50760,10 @@
     </row>
     <row r="10">
       <c r="A10" s="25" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -50779,10 +50793,10 @@
     </row>
     <row r="11">
       <c r="A11" s="25" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
@@ -50827,10 +50841,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -50859,10 +50873,10 @@
     </row>
     <row r="2">
       <c r="A2" s="27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>

</xml_diff>

<commit_message>
Login & Logout deleted in all TC's and Description added to all testcases in jira
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <x:si>
     <x:t>TestCase</x:t>
   </x:si>
@@ -427,7 +427,7 @@
     <x:t>Testcases\TC-2</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02455241</x:t>
+    <x:t>01-0000-02455250</x:t>
   </x:si>
   <x:si>
     <x:t>TC-3</x:t>
@@ -442,9 +442,6 @@
     <x:t>Testcases\TC-4</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02455228</x:t>
-  </x:si>
-  <x:si>
     <x:t>TC-5</x:t>
   </x:si>
   <x:si>
@@ -457,7 +454,7 @@
     <x:t>Testcases\TC-6</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02455229</x:t>
+    <x:t>01-0000-02455232</x:t>
   </x:si>
   <x:si>
     <x:t>TC-7</x:t>
@@ -472,7 +469,7 @@
     <x:t>Testcases\TC-8</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02455230</x:t>
+    <x:t>01-0000-02455252</x:t>
   </x:si>
   <x:si>
     <x:t>TC-9</x:t>
@@ -624,7 +621,7 @@
   <x:borders count="1">
     <x:border/>
   </x:borders>
-  <x:cellStyleXfs count="143">
+  <x:cellStyleXfs count="283">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="1" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -678,6 +675,426 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1485,7 +1902,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="19.73625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="50" width="29.63" style="31" customWidth="1"/>
   </x:cols>
@@ -53707,7 +54124,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="19.73625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="3" width="13.340625" style="31" customWidth="1"/>
     <x:col min="4" max="4" width="24.75" style="31" customWidth="1"/>
@@ -54108,7 +54525,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="19.73625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="2" width="25.63" style="31" customWidth="1"/>
   </x:cols>
@@ -54257,7 +54674,7 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="C5" s="58" t="s">
-        <x:v>141</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D5" s="58" t="s"/>
       <x:c r="E5" s="58" t="s"/>
@@ -54286,10 +54703,10 @@
     </x:row>
     <x:row r="6" spans="1:27">
       <x:c r="A6" s="58" t="s">
-        <x:v>142</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B6" s="58" t="s">
-        <x:v>143</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C6" s="58" t="s"/>
       <x:c r="D6" s="58" t="s"/>
@@ -54319,13 +54736,13 @@
     </x:row>
     <x:row r="7" spans="1:27">
       <x:c r="A7" s="58" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="B7" s="58" t="s">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="B7" s="58" t="s">
+      <x:c r="C7" s="58" t="s">
         <x:v>145</x:v>
-      </x:c>
-      <x:c r="C7" s="58" t="s">
-        <x:v>146</x:v>
       </x:c>
       <x:c r="D7" s="58" t="s"/>
       <x:c r="E7" s="58" t="s"/>
@@ -54354,10 +54771,10 @@
     </x:row>
     <x:row r="8" spans="1:27">
       <x:c r="A8" s="58" t="s">
-        <x:v>147</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B8" s="58" t="s">
-        <x:v>148</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="C8" s="58" t="s"/>
       <x:c r="D8" s="58" t="s"/>
@@ -54387,13 +54804,13 @@
     </x:row>
     <x:row r="9" spans="1:27">
       <x:c r="A9" s="58" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B9" s="58" t="s">
         <x:v>149</x:v>
       </x:c>
-      <x:c r="B9" s="58" t="s">
+      <x:c r="C9" s="58" t="s">
         <x:v>150</x:v>
-      </x:c>
-      <x:c r="C9" s="58" t="s">
-        <x:v>151</x:v>
       </x:c>
       <x:c r="D9" s="58" t="s"/>
       <x:c r="E9" s="58" t="s"/>
@@ -54422,10 +54839,10 @@
     </x:row>
     <x:row r="10" spans="1:27">
       <x:c r="A10" s="58" t="s">
-        <x:v>152</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B10" s="58" t="s">
-        <x:v>153</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C10" s="58" t="s"/>
       <x:c r="D10" s="58" t="s"/>
@@ -54455,10 +54872,10 @@
     </x:row>
     <x:row r="11" spans="1:27">
       <x:c r="A11" s="58" t="s">
-        <x:v>154</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="B11" s="58" t="s">
-        <x:v>155</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C11" s="58" t="s"/>
       <x:c r="D11" s="58" t="s"/>
@@ -54505,14 +54922,14 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="19.73625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
   <x:sheetData>
     <x:row r="1" spans="1:26">
       <x:c r="A1" s="32" t="s">
-        <x:v>156</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B1" s="32" t="s">
-        <x:v>157</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C1" s="32" t="s"/>
       <x:c r="D1" s="32" t="s"/>
@@ -54541,10 +54958,10 @@
     </x:row>
     <x:row r="2" spans="1:26">
       <x:c r="A2" s="46" t="s">
-        <x:v>158</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B2" s="46" t="s">
-        <x:v>157</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C2" s="46" t="s"/>
       <x:c r="D2" s="46" t="s"/>

</xml_diff>

<commit_message>
URL address changes in all TC's
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -427,7 +427,7 @@
     <x:t>Testcases\TC-2</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02455250</x:t>
+    <x:t>01-0000-02455308</x:t>
   </x:si>
   <x:si>
     <x:t>TC-3</x:t>
@@ -440,6 +440,9 @@
   </x:si>
   <x:si>
     <x:t>Testcases\TC-4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-0000-02455301</x:t>
   </x:si>
   <x:si>
     <x:t>TC-5</x:t>
@@ -467,9 +470,6 @@
   </x:si>
   <x:si>
     <x:t>Testcases\TC-8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01-0000-02455252</x:t>
   </x:si>
   <x:si>
     <x:t>TC-9</x:t>
@@ -621,7 +621,7 @@
   <x:borders count="1">
     <x:border/>
   </x:borders>
-  <x:cellStyleXfs count="283">
+  <x:cellStyleXfs count="703">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="1" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -675,6 +675,1266 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1902,7 +3162,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="48.16125" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="50" width="29.63" style="31" customWidth="1"/>
   </x:cols>
@@ -54124,7 +55384,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="48.16125" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="3" width="13.340625" style="31" customWidth="1"/>
     <x:col min="4" max="4" width="24.75" style="31" customWidth="1"/>
@@ -54525,7 +55785,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="48.16125" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="2" width="25.63" style="31" customWidth="1"/>
   </x:cols>
@@ -54674,7 +55934,7 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="C5" s="58" t="s">
-        <x:v>136</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D5" s="58" t="s"/>
       <x:c r="E5" s="58" t="s"/>
@@ -54703,10 +55963,10 @@
     </x:row>
     <x:row r="6" spans="1:27">
       <x:c r="A6" s="58" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B6" s="58" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C6" s="58" t="s"/>
       <x:c r="D6" s="58" t="s"/>
@@ -54736,13 +55996,13 @@
     </x:row>
     <x:row r="7" spans="1:27">
       <x:c r="A7" s="58" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B7" s="58" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="C7" s="58" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D7" s="58" t="s"/>
       <x:c r="E7" s="58" t="s"/>
@@ -54771,10 +56031,10 @@
     </x:row>
     <x:row r="8" spans="1:27">
       <x:c r="A8" s="58" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="B8" s="58" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="C8" s="58" t="s"/>
       <x:c r="D8" s="58" t="s"/>
@@ -54804,13 +56064,13 @@
     </x:row>
     <x:row r="9" spans="1:27">
       <x:c r="A9" s="58" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="B9" s="58" t="s">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="C9" s="58" t="s">
-        <x:v>150</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D9" s="58" t="s"/>
       <x:c r="E9" s="58" t="s"/>
@@ -54922,7 +56182,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="26.8425" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="48.16125" defaultRowHeight="15.75" customHeight="1"/>
   <x:sheetData>
     <x:row r="1" spans="1:26">
       <x:c r="A1" s="32" t="s">

</xml_diff>

<commit_message>
Changes in search box
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <x:si>
     <x:t>TestCase</x:t>
   </x:si>
@@ -434,7 +434,7 @@
     <x:t>Testcases\TC-2</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456083</x:t>
+    <x:t>01-0000-02456098</x:t>
   </x:si>
   <x:si>
     <x:t>TC-3</x:t>
@@ -464,6 +464,9 @@
     <x:t>Testcases\TC-8</x:t>
   </x:si>
   <x:si>
+    <x:t>01-0000-02456140</x:t>
+  </x:si>
+  <x:si>
     <x:t>TC-9</x:t>
   </x:si>
   <x:si>
@@ -474,6 +477,9 @@
   </x:si>
   <x:si>
     <x:t>Testcases\TC-10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-0000-02456099</x:t>
   </x:si>
   <x:si>
     <x:t>username</x:t>
@@ -602,7 +608,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="42">
+  <x:cellStyleXfs count="94">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -614,6 +620,162 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1056,7 +1218,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="87.2725" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="50" width="29.570312" style="18" customWidth="1"/>
   </x:cols>
@@ -53277,7 +53439,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="87.2725" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="3" width="13.285156" style="18" customWidth="1"/>
     <x:col min="4" max="4" width="24.710938" style="18" customWidth="1"/>
@@ -53669,7 +53831,7 @@
       <x:selection activeCell="C17" sqref="C17 C17:C17"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="87.2725" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="2" width="25.570312" style="18" customWidth="1"/>
   </x:cols>
@@ -53886,7 +54048,7 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="C7" s="31" t="s">
-        <x:v>141</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D7" s="31" t="s"/>
       <x:c r="E7" s="31" t="s"/>
@@ -53915,10 +54077,10 @@
     </x:row>
     <x:row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A8" s="31" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="B8" s="31" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="C8" s="31" t="s"/>
       <x:c r="D8" s="31" t="s"/>
@@ -53948,13 +54110,13 @@
     </x:row>
     <x:row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A9" s="31" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="B9" s="31" t="s">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="C9" s="31" t="s">
-        <x:v>141</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D9" s="31" t="s"/>
       <x:c r="E9" s="31" t="s"/>
@@ -54002,14 +54164,14 @@
       <x:selection activeCell="A11" sqref="A11 A11:A11"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="87.2725" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:sheetData>
     <x:row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A1" s="19" t="s">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B1" s="19" t="s">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C1" s="19" t="s"/>
       <x:c r="D1" s="19" t="s"/>
@@ -54038,10 +54200,10 @@
     </x:row>
     <x:row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A2" s="32" t="s">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B2" s="32" t="s">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C2" s="32" t="s"/>
       <x:c r="D2" s="32" t="s"/>
@@ -54070,13 +54232,13 @@
     </x:row>
     <x:row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A7" s="31" t="s">
-        <x:v>153</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B7" s="31" t="s">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C7" s="31" t="s">
-        <x:v>155</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="D7" s="31" t="s"/>
       <x:c r="E7" s="31" t="s"/>
@@ -54105,10 +54267,10 @@
     </x:row>
     <x:row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A9" s="31" t="s">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B9" s="31" t="s">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="C9" s="31" t="s"/>
       <x:c r="D9" s="31" t="s"/>

</xml_diff>

<commit_message>
Changes in TC-6 & 9
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -434,7 +434,7 @@
     <x:t>Testcases\TC-2</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456098</x:t>
+    <x:t>01-0000-02456189</x:t>
   </x:si>
   <x:si>
     <x:t>TC-3</x:t>
@@ -464,7 +464,7 @@
     <x:t>Testcases\TC-8</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456140</x:t>
+    <x:t>01-0000-02456209</x:t>
   </x:si>
   <x:si>
     <x:t>TC-9</x:t>
@@ -479,7 +479,7 @@
     <x:t>Testcases\TC-10</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456099</x:t>
+    <x:t>01-0000-02456190</x:t>
   </x:si>
   <x:si>
     <x:t>username</x:t>
@@ -608,7 +608,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="94">
+  <x:cellStyleXfs count="224">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -620,6 +620,396 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1218,7 +1608,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="50" width="29.570312" style="18" customWidth="1"/>
   </x:cols>
@@ -53439,7 +53829,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="3" width="13.285156" style="18" customWidth="1"/>
     <x:col min="4" max="4" width="24.710938" style="18" customWidth="1"/>
@@ -53831,7 +54221,7 @@
       <x:selection activeCell="C17" sqref="C17 C17:C17"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="2" width="25.570312" style="18" customWidth="1"/>
   </x:cols>
@@ -54164,7 +54554,7 @@
       <x:selection activeCell="A11" sqref="A11 A11:A11"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="90.115" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:sheetData>
     <x:row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A1" s="19" t="s">

</xml_diff>

<commit_message>
Changes in TC-6&8 validations
</commit_message>
<xml_diff>
--- a/Config/credential sheet.xlsx
+++ b/Config/credential sheet.xlsx
@@ -434,7 +434,7 @@
     <x:t>Testcases\TC-2</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456189</x:t>
+    <x:t>01-0000-02456246</x:t>
   </x:si>
   <x:si>
     <x:t>TC-3</x:t>
@@ -464,7 +464,7 @@
     <x:t>Testcases\TC-8</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456209</x:t>
+    <x:t>01-0000-02456253</x:t>
   </x:si>
   <x:si>
     <x:t>TC-9</x:t>
@@ -479,7 +479,7 @@
     <x:t>Testcases\TC-10</x:t>
   </x:si>
   <x:si>
-    <x:t>01-0000-02456190</x:t>
+    <x:t>01-0000-02456247</x:t>
   </x:si>
   <x:si>
     <x:t>username</x:t>
@@ -608,7 +608,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="224">
+  <x:cellStyleXfs count="328">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -620,6 +620,318 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1608,7 +1920,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="102.90625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="50" width="29.570312" style="18" customWidth="1"/>
   </x:cols>
@@ -53829,7 +54141,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="102.90625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="3" width="13.285156" style="18" customWidth="1"/>
     <x:col min="4" max="4" width="24.710938" style="18" customWidth="1"/>
@@ -54221,7 +54533,7 @@
       <x:selection activeCell="C17" sqref="C17 C17:C17"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="102.90625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="2" width="25.570312" style="18" customWidth="1"/>
   </x:cols>
@@ -54554,7 +54866,7 @@
       <x:selection activeCell="A11" sqref="A11 A11:A11"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="97.22125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="102.90625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <x:sheetData>
     <x:row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <x:c r="A1" s="19" t="s">

</xml_diff>